<commit_message>
format match to others, link to production code
</commit_message>
<xml_diff>
--- a/data/verification/samples_clustering_runtime_memory.xlsx
+++ b/data/verification/samples_clustering_runtime_memory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="500" windowWidth="25860" windowHeight="28220" tabRatio="500"/>
+    <workbookView xWindow="9900" yWindow="460" windowWidth="25860" windowHeight="28220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>samples</t>
   </si>
@@ -78,12 +78,6 @@
   </si>
   <si>
     <t>sample_random</t>
-  </si>
-  <si>
-    <t>Size/MB</t>
-  </si>
-  <si>
-    <t>name_size</t>
   </si>
   <si>
     <t>genes_lookup_table</t>
@@ -170,11 +164,41 @@
   <si>
     <t>h_mat</t>
   </si>
+  <si>
+    <t>45b724b</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>Bytes</t>
+  </si>
+  <si>
+    <t>gene name string</t>
+  </si>
+  <si>
+    <t>sample name string</t>
+  </si>
+  <si>
+    <t>letters</t>
+  </si>
+  <si>
+    <t>items</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>production version</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -240,12 +264,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -274,11 +299,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -554,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="198" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="198" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -566,758 +595,794 @@
     <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" style="6" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" style="13" customWidth="1"/>
     <col min="6" max="6" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <f>1000000</f>
         <v>1000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
+      <c r="C3" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>4</v>
+      <c r="C4" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>32</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="E7">
+      <c r="C7" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="13">
         <f>5*60/24</f>
         <v>12.5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>248</v>
-      </c>
-      <c r="C8" s="6">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>17547</v>
-      </c>
-      <c r="C9" s="6">
-        <f>15*B4</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>289432</v>
-      </c>
-      <c r="C10" s="6">
-        <f>15*B4</f>
-        <v>60</v>
-      </c>
-    </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>11128</v>
-      </c>
-      <c r="C11" s="6">
-        <v>15</v>
+        <v>248</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>17547</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>289432</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>11128</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="8">
+        <f>(E43+E50*(B15+1))</f>
+        <v>301.98581599999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="8">
-        <f>(E40+E47*(B12+1))</f>
-        <v>301.98581599999994</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>174</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="11">
-        <f>((B9+1)*(B8+1)*B6)/B2</f>
-        <v>34.955615999999999</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="12">
-        <f>C16*D16</f>
-        <v>34.955615999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>175</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="11">
-        <f>(B10+1)*3*B6/B2</f>
-        <v>6.9463920000000003</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="12">
-        <f t="shared" ref="E17:E39" si="0">C17*D17</f>
-        <v>6.9463920000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>177</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="11">
-        <f>(B11*C11*B4)/B2</f>
-        <v>0.66768000000000005</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="12">
-        <f t="shared" si="0"/>
-        <v>0.66768000000000005</v>
+      <c r="E18" s="13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C19" s="11">
-        <f>(B11*C11*B4)/B2</f>
-        <v>0.66768000000000005</v>
+        <f>((B12+1)*(B11+1)*B9)/B3</f>
+        <v>34.955615999999999</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19" s="12">
-        <f t="shared" si="0"/>
-        <v>0.66768000000000005</v>
+      <c r="E19" s="13">
+        <f>C19*D19</f>
+        <v>34.955615999999999</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C20" s="11">
-        <f>(B11*C11*B4)/B2</f>
-        <v>0.66768000000000005</v>
+        <f>(B13+1)*3*B9/B3</f>
+        <v>6.9463920000000003</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="12">
-        <f t="shared" si="0"/>
-        <v>0.66768000000000005</v>
+      <c r="E20" s="13">
+        <f t="shared" ref="E20:E42" si="0">C20*D20</f>
+        <v>6.9463920000000003</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C21" s="11">
-        <f>(B11*C11*B4+B11*B6)/B2</f>
-        <v>0.75670400000000004</v>
+        <f>(B14*B6*B7)/B3</f>
+        <v>0.66768000000000005</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" s="12">
-        <f t="shared" si="0"/>
-        <v>0.75670400000000004</v>
+      <c r="E21" s="13">
+        <f t="shared" si="0"/>
+        <v>0.66768000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C22" s="11">
-        <f>(B10+1)*3*B6/B2</f>
-        <v>6.9463920000000003</v>
+        <f>(B14*B6*B7)/B3</f>
+        <v>0.66768000000000005</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" s="12">
-        <f t="shared" si="0"/>
-        <v>6.9463920000000003</v>
+      <c r="E22" s="13">
+        <f t="shared" si="0"/>
+        <v>0.66768000000000005</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C23" s="11">
-        <f>(B10+1)*3*B6/B2</f>
-        <v>6.9463920000000003</v>
+        <f>(B14*B6*B7)/B3</f>
+        <v>0.66768000000000005</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" s="12">
-        <f t="shared" si="0"/>
-        <v>6.9463920000000003</v>
+      <c r="E23" s="13">
+        <f t="shared" si="0"/>
+        <v>0.66768000000000005</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C24" s="11">
-        <f>2*(B10+1)*3*B6/B2</f>
-        <v>13.892784000000001</v>
+        <f>(B14*B6*B7+B14*B9)/B3</f>
+        <v>0.75670400000000004</v>
       </c>
       <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24" s="12">
-        <f t="shared" si="0"/>
-        <v>27.785568000000001</v>
+        <v>1</v>
+      </c>
+      <c r="E24" s="13">
+        <f t="shared" si="0"/>
+        <v>0.75670400000000004</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C25" s="11">
-        <f>(B10*2*B7+B10*B6)/B2</f>
-        <v>4.6309120000000004</v>
+        <f>(B13+1)*3*B9/B3</f>
+        <v>6.9463920000000003</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="E25" s="12">
-        <f t="shared" si="0"/>
-        <v>4.6309120000000004</v>
+      <c r="E25" s="13">
+        <f t="shared" si="0"/>
+        <v>6.9463920000000003</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C26" s="11">
-        <f>(B10*2*B7+B10*B6)/B2</f>
-        <v>4.6309120000000004</v>
+        <f>(B13+1)*3*B9/B3</f>
+        <v>6.9463920000000003</v>
       </c>
       <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26" s="12">
-        <f t="shared" si="0"/>
-        <v>9.2618240000000007</v>
+        <v>1</v>
+      </c>
+      <c r="E26" s="13">
+        <f t="shared" si="0"/>
+        <v>6.9463920000000003</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C27" s="11">
-        <f>(B11*B6)/B2</f>
-        <v>8.9024000000000006E-2</v>
+        <f>2*(B13+1)*3*B9/B3</f>
+        <v>13.892784000000001</v>
       </c>
       <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" s="12">
-        <f t="shared" si="0"/>
-        <v>8.9024000000000006E-2</v>
+        <v>2</v>
+      </c>
+      <c r="E27" s="13">
+        <f t="shared" si="0"/>
+        <v>27.785568000000001</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C28" s="11">
-        <f>(B10*2*B7+B10*B6)/B2</f>
+        <f>(B13*2*B10+B13*B9)/B3</f>
         <v>4.6309120000000004</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="13">
         <f t="shared" si="0"/>
         <v>4.6309120000000004</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C29" s="11">
-        <f>((B11+1)*(B8+1)*B6)/B2</f>
-        <v>22.168968</v>
+        <f>(B13*2*B10+B13*B9)/B3</f>
+        <v>4.6309120000000004</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
-      <c r="E29" s="12">
-        <f t="shared" si="0"/>
-        <v>44.337935999999999</v>
+      <c r="E29" s="13">
+        <f t="shared" si="0"/>
+        <v>9.2618240000000007</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C30" s="11">
-        <f>(B11*B8*B6)/B2</f>
-        <v>22.077952</v>
+        <f>(B14*B9)/B3</f>
+        <v>8.9024000000000006E-2</v>
       </c>
       <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="E30" s="12">
-        <f t="shared" si="0"/>
-        <v>44.155904</v>
+        <v>1</v>
+      </c>
+      <c r="E30" s="13">
+        <f t="shared" si="0"/>
+        <v>8.9024000000000006E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C31" s="11">
-        <f>(B8*C8*B4)/B2</f>
-        <v>3.1744000000000001E-2</v>
+        <f>(B13*2*B10+B13*B9)/B3</f>
+        <v>4.6309120000000004</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31" s="12">
-        <f t="shared" si="0"/>
-        <v>3.1744000000000001E-2</v>
+      <c r="E31" s="13">
+        <f t="shared" si="0"/>
+        <v>4.6309120000000004</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="C32" s="11">
+        <f>((B14+1)*(B11+1)*B9)/B3</f>
+        <v>22.168968</v>
+      </c>
       <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="E32" s="13">
+        <f t="shared" si="0"/>
+        <v>44.337935999999999</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>234</v>
+        <v>192</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C33" s="11">
-        <f>(B8*B8*B6)/B2</f>
-        <v>0.49203200000000002</v>
+        <f>(B14*B11*B9)/B3</f>
+        <v>22.077952</v>
       </c>
       <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33" s="12">
-        <f t="shared" si="0"/>
-        <v>0.49203200000000002</v>
+        <v>2</v>
+      </c>
+      <c r="E33" s="13">
+        <f t="shared" si="0"/>
+        <v>44.155904</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>235</v>
+        <v>193</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C34" s="11">
-        <f>(B8*B8*B6)/B2</f>
-        <v>0.49203200000000002</v>
+        <f>(B11*B5*B7)/B3</f>
+        <v>3.1744000000000001E-2</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="E34" s="12">
-        <f t="shared" si="0"/>
-        <v>0.49203200000000002</v>
+      <c r="E34" s="13">
+        <f t="shared" si="0"/>
+        <v>3.1744000000000001E-2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="11">
-        <f>(B8*B8*B6)/B2</f>
-        <v>0.49203200000000002</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C35" s="11"/>
       <c r="D35">
         <v>1</v>
       </c>
-      <c r="E35" s="12">
-        <f t="shared" si="0"/>
-        <v>0.49203200000000002</v>
+      <c r="E35" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C36" s="11">
-        <f>3*(B8*B5)/B2</f>
-        <v>5.9519999999999998E-3</v>
+        <f>(B11*B11*B9)/B3</f>
+        <v>0.49203200000000002</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
-      <c r="E36" s="12">
-        <f t="shared" si="0"/>
-        <v>5.9519999999999998E-3</v>
+      <c r="E36" s="13">
+        <f t="shared" si="0"/>
+        <v>0.49203200000000002</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="C37" s="11">
+        <f>(B11*B11*B9)/B3</f>
+        <v>0.49203200000000002</v>
+      </c>
       <c r="D37">
         <v>1</v>
       </c>
-      <c r="E37" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="E37" s="13">
+        <f t="shared" si="0"/>
+        <v>0.49203200000000002</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="C38" s="11">
+        <f>(B11*B11*B9)/B3</f>
+        <v>0.49203200000000002</v>
+      </c>
       <c r="D38">
         <v>1</v>
       </c>
-      <c r="E38" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="E38" s="13">
+        <f t="shared" si="0"/>
+        <v>0.49203200000000002</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
+        <v>237</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="11">
+        <f>3*(B11*B8)/B3</f>
+        <v>5.9519999999999998E-3</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" s="13">
+        <f t="shared" si="0"/>
+        <v>5.9519999999999998E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>239</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="11"/>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>240</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="11"/>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
         <v>241</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B42" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="11"/>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="11"/>
+      <c r="D43"/>
+      <c r="E43" s="13">
+        <f>SUM(E19:E42)</f>
+        <v>194.96040799999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="4"/>
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="C46" s="11">
+        <f>(C29+C33+C30+C31)</f>
+        <v>31.428799999999995</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" s="13">
+        <f>C46*D46</f>
+        <v>31.428799999999995</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="7">
+        <v>353</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="11">
+        <f>C33</f>
+        <v>22.077952</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" s="13">
+        <f t="shared" ref="E47:E48" si="1">C47*D47</f>
+        <v>22.077952</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="7">
+        <v>356</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="11"/>
-      <c r="D40"/>
-      <c r="E40" s="12">
-        <f>SUM(E16:E39)</f>
-        <v>194.96040799999997</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="4"/>
-      <c r="D41"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="4"/>
-      <c r="D42"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="11">
-        <f>(C26+C30+C27+C28)</f>
-        <v>31.428799999999995</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43" s="12">
-        <f>C43*D43</f>
-        <v>31.428799999999995</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="7">
-        <v>353</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" s="11">
-        <f>C30</f>
-        <v>22.077952</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" s="12">
-        <f t="shared" ref="E44:E45" si="1">C44*D44</f>
-        <v>22.077952</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="7">
-        <v>356</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C45" s="11">
-        <f>3*B8*B6/B2</f>
+      <c r="C48" s="11">
+        <f>3*B11*B9/B3</f>
         <v>5.9519999999999998E-3</v>
       </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45" s="12">
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" s="13">
         <f t="shared" si="1"/>
         <v>5.9519999999999998E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B46" s="4"/>
-      <c r="C46" s="11"/>
-      <c r="D46"/>
-      <c r="E46" s="12"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="11"/>
-      <c r="D47"/>
-      <c r="E47" s="12">
-        <f>SUM(E43:E46)</f>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="4"/>
+      <c r="C49" s="11"/>
+      <c r="D49"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="4"/>
+      <c r="C50" s="11"/>
+      <c r="D50"/>
+      <c r="E50" s="13">
+        <f>SUM(E46:E49)</f>
         <v>53.512703999999992</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="4"/>
-      <c r="D48"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="4"/>
-      <c r="D49"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B50" s="4"/>
-      <c r="D50"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B51" s="4"/>
       <c r="D51"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B52" s="4"/>
       <c r="D52"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B53" s="4"/>
       <c r="D53"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B54" s="4"/>
       <c r="D54"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
       <c r="D55"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
       <c r="D56"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B57" s="4"/>
       <c r="D57"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
       <c r="D58"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
       <c r="D59"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
       <c r="D60"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
       <c r="D61"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
       <c r="D62"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
       <c r="D63"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
       <c r="D64"/>
     </row>
@@ -1341,7 +1406,7 @@
       <c r="B69" s="4"/>
       <c r="D69"/>
     </row>
-    <row r="70" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B70" s="4"/>
       <c r="D70"/>
     </row>
@@ -1353,21 +1418,21 @@
       <c r="B72" s="4"/>
       <c r="D72"/>
     </row>
-    <row r="73" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="4"/>
       <c r="D73"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B74" s="4"/>
-      <c r="D74" s="1"/>
+      <c r="D74"/>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B75" s="4"/>
-      <c r="D75" s="1"/>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D75"/>
+    </row>
+    <row r="76" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="4"/>
-      <c r="D76" s="1"/>
+      <c r="D76"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B77" s="4"/>
@@ -1385,10 +1450,25 @@
       <c r="B80" s="4"/>
       <c r="D80" s="1"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" s="4"/>
+      <c r="D81" s="1"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B82" s="4"/>
+      <c r="D82" s="1"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B83" s="4"/>
+      <c r="D83" s="1"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B84" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>